<commit_message>
Atualização automática JSON e J1BNFE.xlsx
</commit_message>
<xml_diff>
--- a/src/data/J1BNFE.xlsx
+++ b/src/data/J1BNFE.xlsx
@@ -40,6 +40,9 @@
     <t>Hora processamento</t>
   </si>
   <si>
+    <t>10489</t>
+  </si>
+  <si>
     <t>536</t>
   </si>
   <si>
@@ -121,9 +124,6 @@
     <t>894</t>
   </si>
   <si>
-    <t>10489</t>
-  </si>
-  <si>
     <t>913</t>
   </si>
   <si>
@@ -685,6 +685,27 @@
     <t>5650</t>
   </si>
   <si>
+    <t>9972</t>
+  </si>
+  <si>
+    <t>10494</t>
+  </si>
+  <si>
+    <t>10542</t>
+  </si>
+  <si>
+    <t>10538</t>
+  </si>
+  <si>
+    <t>10601</t>
+  </si>
+  <si>
+    <t>10617</t>
+  </si>
+  <si>
+    <t>10618</t>
+  </si>
+  <si>
     <t>5667</t>
   </si>
   <si>
@@ -694,27 +715,6 @@
     <t>5733</t>
   </si>
   <si>
-    <t>9972</t>
-  </si>
-  <si>
-    <t>10494</t>
-  </si>
-  <si>
-    <t>10542</t>
-  </si>
-  <si>
-    <t>10538</t>
-  </si>
-  <si>
-    <t>10601</t>
-  </si>
-  <si>
-    <t>10617</t>
-  </si>
-  <si>
-    <t>10618</t>
-  </si>
-  <si>
     <t>5739</t>
   </si>
   <si>
@@ -1300,6 +1300,9 @@
     <t>X</t>
   </si>
   <si>
+    <t>000000291</t>
+  </si>
+  <si>
     <t>000000002</t>
   </si>
   <si>
@@ -1357,9 +1360,6 @@
     <t>000000030</t>
   </si>
   <si>
-    <t>000000291</t>
-  </si>
-  <si>
     <t>000000032</t>
   </si>
   <si>
@@ -1747,6 +1747,21 @@
     <t>000000154</t>
   </si>
   <si>
+    <t>000000278</t>
+  </si>
+  <si>
+    <t>000000292</t>
+  </si>
+  <si>
+    <t>000000293</t>
+  </si>
+  <si>
+    <t>000000294</t>
+  </si>
+  <si>
+    <t>000000295</t>
+  </si>
+  <si>
     <t>000000155</t>
   </si>
   <si>
@@ -1756,21 +1771,6 @@
     <t>000000157</t>
   </si>
   <si>
-    <t>000000278</t>
-  </si>
-  <si>
-    <t>000000292</t>
-  </si>
-  <si>
-    <t>000000293</t>
-  </si>
-  <si>
-    <t>000000294</t>
-  </si>
-  <si>
-    <t>000000295</t>
-  </si>
-  <si>
     <t>000000158</t>
   </si>
   <si>
@@ -2167,6 +2167,9 @@
     <t>000000290</t>
   </si>
   <si>
+    <t>2026-02-24 00:00:00</t>
+  </si>
+  <si>
     <t>2026-02-01 00:00:00</t>
   </si>
   <si>
@@ -2176,9 +2179,6 @@
     <t>2026-02-03 00:00:00</t>
   </si>
   <si>
-    <t>2026-02-24 00:00:00</t>
-  </si>
-  <si>
     <t>2026-02-04 00:00:00</t>
   </si>
   <si>
@@ -2248,6 +2248,9 @@
     <t>Cancelamento por problemas técnicos</t>
   </si>
   <si>
+    <t>WENDRYO.G</t>
+  </si>
+  <si>
     <t>MANOEL.F</t>
   </si>
   <si>
@@ -2257,15 +2260,15 @@
     <t>IURI.C</t>
   </si>
   <si>
-    <t>WENDRYO.G</t>
-  </si>
-  <si>
     <t>CLEITON.C</t>
   </si>
   <si>
     <t>ANA.V</t>
   </si>
   <si>
+    <t>07:31:03</t>
+  </si>
+  <si>
     <t>14:21:32</t>
   </si>
   <si>
@@ -2332,9 +2335,6 @@
     <t>09:19:52</t>
   </si>
   <si>
-    <t>07:31:03</t>
-  </si>
-  <si>
     <t>09:42:10</t>
   </si>
   <si>
@@ -2860,6 +2860,24 @@
     <t>08:08:13</t>
   </si>
   <si>
+    <t>07:46:31</t>
+  </si>
+  <si>
+    <t>08:30:33</t>
+  </si>
+  <si>
+    <t>08:31:27</t>
+  </si>
+  <si>
+    <t>09:23:17</t>
+  </si>
+  <si>
+    <t>09:39:58</t>
+  </si>
+  <si>
+    <t>09:40:14</t>
+  </si>
+  <si>
     <t>08:26:24</t>
   </si>
   <si>
@@ -2867,24 +2885,6 @@
   </si>
   <si>
     <t>09:13:43</t>
-  </si>
-  <si>
-    <t>07:46:31</t>
-  </si>
-  <si>
-    <t>08:30:33</t>
-  </si>
-  <si>
-    <t>08:31:27</t>
-  </si>
-  <si>
-    <t>09:23:17</t>
-  </si>
-  <si>
-    <t>09:39:58</t>
-  </si>
-  <si>
-    <t>09:40:14</t>
   </si>
   <si>
     <t>09:18:56</t>
@@ -3788,7 +3788,7 @@
         <v>429</v>
       </c>
       <c r="E3" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="G3" t="s">
         <v>745</v>
@@ -3801,23 +3801,14 @@
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
-        <v>426</v>
-      </c>
-      <c r="C4" t="s">
-        <v>427</v>
-      </c>
       <c r="D4" t="s">
         <v>430</v>
       </c>
       <c r="E4" t="s">
-        <v>717</v>
-      </c>
-      <c r="F4" t="s">
-        <v>741</v>
+        <v>718</v>
       </c>
       <c r="G4" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="H4" t="s">
         <v>752</v>
@@ -3837,16 +3828,16 @@
         <v>431</v>
       </c>
       <c r="E5" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="F5" t="s">
         <v>741</v>
       </c>
       <c r="G5" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="H5" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -3860,19 +3851,19 @@
         <v>427</v>
       </c>
       <c r="D6" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="E6" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="F6" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="G6" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="H6" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -3886,19 +3877,19 @@
         <v>427</v>
       </c>
       <c r="D7" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E7" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="F7" t="s">
         <v>742</v>
       </c>
       <c r="G7" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="H7" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -3915,30 +3906,39 @@
         <v>433</v>
       </c>
       <c r="E8" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="F8" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="G8" t="s">
         <v>745</v>
       </c>
       <c r="H8" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>15</v>
       </c>
+      <c r="B9" t="s">
+        <v>426</v>
+      </c>
+      <c r="C9" t="s">
+        <v>427</v>
+      </c>
       <c r="D9" t="s">
         <v>434</v>
       </c>
       <c r="E9" t="s">
         <v>718</v>
       </c>
+      <c r="F9" t="s">
+        <v>741</v>
+      </c>
       <c r="G9" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="H9" t="s">
         <v>753</v>
@@ -3948,43 +3948,43 @@
       <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s">
-        <v>426</v>
-      </c>
-      <c r="C10" t="s">
-        <v>427</v>
-      </c>
       <c r="D10" t="s">
         <v>435</v>
       </c>
       <c r="E10" t="s">
-        <v>718</v>
-      </c>
-      <c r="F10" t="s">
-        <v>741</v>
+        <v>719</v>
       </c>
       <c r="G10" t="s">
         <v>744</v>
       </c>
       <c r="H10" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>17</v>
       </c>
+      <c r="B11" t="s">
+        <v>426</v>
+      </c>
+      <c r="C11" t="s">
+        <v>427</v>
+      </c>
       <c r="D11" t="s">
         <v>436</v>
       </c>
       <c r="E11" t="s">
-        <v>718</v>
+        <v>719</v>
+      </c>
+      <c r="F11" t="s">
+        <v>741</v>
       </c>
       <c r="G11" t="s">
         <v>745</v>
       </c>
       <c r="H11" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -3995,10 +3995,10 @@
         <v>437</v>
       </c>
       <c r="E12" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="G12" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="H12" t="s">
         <v>755</v>
@@ -4009,13 +4009,13 @@
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>430</v>
+        <v>438</v>
       </c>
       <c r="E13" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="G13" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="H13" t="s">
         <v>756</v>
@@ -4026,10 +4026,10 @@
         <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="E14" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="G14" t="s">
         <v>746</v>
@@ -4042,17 +4042,14 @@
       <c r="A15" t="s">
         <v>21</v>
       </c>
-      <c r="B15" t="s">
-        <v>426</v>
-      </c>
       <c r="D15" t="s">
         <v>439</v>
       </c>
       <c r="E15" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="G15" t="s">
-        <v>744</v>
+        <v>747</v>
       </c>
       <c r="H15" t="s">
         <v>758</v>
@@ -4062,6 +4059,9 @@
       <c r="A16" t="s">
         <v>22</v>
       </c>
+      <c r="B16" t="s">
+        <v>426</v>
+      </c>
       <c r="D16" t="s">
         <v>440</v>
       </c>
@@ -4083,7 +4083,7 @@
         <v>441</v>
       </c>
       <c r="E17" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="G17" t="s">
         <v>746</v>
@@ -4097,13 +4097,13 @@
         <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>431</v>
+        <v>442</v>
       </c>
       <c r="E18" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="G18" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="H18" t="s">
         <v>761</v>
@@ -4114,13 +4114,13 @@
         <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="E19" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="G19" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H19" t="s">
         <v>762</v>
@@ -4131,10 +4131,10 @@
         <v>26</v>
       </c>
       <c r="D20" t="s">
-        <v>429</v>
+        <v>440</v>
       </c>
       <c r="E20" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="G20" t="s">
         <v>746</v>
@@ -4148,10 +4148,10 @@
         <v>27</v>
       </c>
       <c r="D21" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E21" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="G21" t="s">
         <v>747</v>
@@ -4165,13 +4165,13 @@
         <v>28</v>
       </c>
       <c r="D22" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="E22" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="G22" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="H22" t="s">
         <v>765</v>
@@ -4182,10 +4182,10 @@
         <v>29</v>
       </c>
       <c r="D23" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E23" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="G23" t="s">
         <v>747</v>
@@ -4202,7 +4202,7 @@
         <v>443</v>
       </c>
       <c r="E24" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="G24" t="s">
         <v>744</v>
@@ -4219,10 +4219,10 @@
         <v>444</v>
       </c>
       <c r="E25" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="G25" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="H25" t="s">
         <v>768</v>
@@ -4236,7 +4236,7 @@
         <v>445</v>
       </c>
       <c r="E26" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="G26" t="s">
         <v>745</v>
@@ -4253,10 +4253,10 @@
         <v>446</v>
       </c>
       <c r="E27" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="G27" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="H27" t="s">
         <v>770</v>
@@ -4267,7 +4267,7 @@
         <v>34</v>
       </c>
       <c r="D28" t="s">
-        <v>433</v>
+        <v>447</v>
       </c>
       <c r="E28" t="s">
         <v>719</v>
@@ -4284,13 +4284,13 @@
         <v>35</v>
       </c>
       <c r="D29" t="s">
-        <v>447</v>
+        <v>434</v>
       </c>
       <c r="E29" t="s">
         <v>720</v>
       </c>
       <c r="G29" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="H29" t="s">
         <v>772</v>
@@ -4304,10 +4304,10 @@
         <v>448</v>
       </c>
       <c r="E30" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="G30" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H30" t="s">
         <v>773</v>
@@ -4321,10 +4321,10 @@
         <v>449</v>
       </c>
       <c r="E31" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="G31" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H31" t="s">
         <v>774</v>
@@ -4338,10 +4338,10 @@
         <v>450</v>
       </c>
       <c r="E32" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="G32" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H32" t="s">
         <v>775</v>
@@ -4355,10 +4355,10 @@
         <v>451</v>
       </c>
       <c r="E33" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="G33" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H33" t="s">
         <v>776</v>
@@ -4372,10 +4372,10 @@
         <v>452</v>
       </c>
       <c r="E34" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="G34" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H34" t="s">
         <v>777</v>
@@ -4392,19 +4392,19 @@
         <v>427</v>
       </c>
       <c r="D35" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="E35" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="F35" t="s">
         <v>741</v>
       </c>
       <c r="G35" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H35" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -4421,16 +4421,16 @@
         <v>453</v>
       </c>
       <c r="E36" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="F36" t="s">
         <v>741</v>
       </c>
       <c r="G36" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H36" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -4438,13 +4438,13 @@
         <v>43</v>
       </c>
       <c r="D37" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="E37" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="G37" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H37" t="s">
         <v>778</v>
@@ -4455,13 +4455,13 @@
         <v>44</v>
       </c>
       <c r="D38" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="E38" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="G38" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H38" t="s">
         <v>779</v>
@@ -4475,10 +4475,10 @@
         <v>454</v>
       </c>
       <c r="E39" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="G39" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H39" t="s">
         <v>780</v>
@@ -4489,13 +4489,13 @@
         <v>46</v>
       </c>
       <c r="D40" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="E40" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="G40" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H40" t="s">
         <v>781</v>
@@ -4509,10 +4509,10 @@
         <v>455</v>
       </c>
       <c r="E41" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="G41" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H41" t="s">
         <v>782</v>
@@ -4526,10 +4526,10 @@
         <v>456</v>
       </c>
       <c r="E42" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="G42" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H42" t="s">
         <v>783</v>
@@ -4549,16 +4549,16 @@
         <v>457</v>
       </c>
       <c r="E43" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="F43" t="s">
         <v>741</v>
       </c>
       <c r="G43" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H43" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -4569,10 +4569,10 @@
         <v>458</v>
       </c>
       <c r="E44" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="G44" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H44" t="s">
         <v>784</v>
@@ -4586,10 +4586,10 @@
         <v>459</v>
       </c>
       <c r="E45" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="G45" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H45" t="s">
         <v>785</v>
@@ -4603,10 +4603,10 @@
         <v>453</v>
       </c>
       <c r="E46" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="G46" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H46" t="s">
         <v>786</v>
@@ -4617,13 +4617,13 @@
         <v>53</v>
       </c>
       <c r="D47" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="E47" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="G47" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H47" t="s">
         <v>787</v>
@@ -4634,13 +4634,13 @@
         <v>54</v>
       </c>
       <c r="D48" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="E48" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="G48" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H48" t="s">
         <v>788</v>
@@ -4654,10 +4654,10 @@
         <v>460</v>
       </c>
       <c r="E49" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="G49" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H49" t="s">
         <v>789</v>
@@ -4671,10 +4671,10 @@
         <v>461</v>
       </c>
       <c r="E50" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="G50" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H50" t="s">
         <v>790</v>
@@ -4688,7 +4688,7 @@
         <v>462</v>
       </c>
       <c r="E51" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="G51" t="s">
         <v>748</v>
@@ -4705,10 +4705,10 @@
         <v>463</v>
       </c>
       <c r="E52" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="G52" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H52" t="s">
         <v>792</v>
@@ -4722,10 +4722,10 @@
         <v>454</v>
       </c>
       <c r="E53" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="G53" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H53" t="s">
         <v>793</v>
@@ -4739,10 +4739,10 @@
         <v>464</v>
       </c>
       <c r="E54" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="G54" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H54" t="s">
         <v>794</v>
@@ -4756,10 +4756,10 @@
         <v>465</v>
       </c>
       <c r="E55" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="G55" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H55" t="s">
         <v>795</v>
@@ -4776,7 +4776,7 @@
         <v>721</v>
       </c>
       <c r="G56" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H56" t="s">
         <v>796</v>
@@ -4793,7 +4793,7 @@
         <v>721</v>
       </c>
       <c r="G57" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H57" t="s">
         <v>797</v>
@@ -4804,13 +4804,13 @@
         <v>64</v>
       </c>
       <c r="D58" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="E58" t="s">
         <v>721</v>
       </c>
       <c r="G58" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H58" t="s">
         <v>798</v>
@@ -4821,13 +4821,13 @@
         <v>65</v>
       </c>
       <c r="D59" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="E59" t="s">
         <v>721</v>
       </c>
       <c r="G59" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H59" t="s">
         <v>799</v>
@@ -4844,7 +4844,7 @@
         <v>721</v>
       </c>
       <c r="G60" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H60" t="s">
         <v>800</v>
@@ -4861,7 +4861,7 @@
         <v>721</v>
       </c>
       <c r="G61" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H61" t="s">
         <v>801</v>
@@ -4878,7 +4878,7 @@
         <v>721</v>
       </c>
       <c r="G62" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H62" t="s">
         <v>802</v>
@@ -4895,7 +4895,7 @@
         <v>427</v>
       </c>
       <c r="D63" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="E63" t="s">
         <v>721</v>
@@ -4904,10 +4904,10 @@
         <v>741</v>
       </c>
       <c r="G63" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H63" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -4915,13 +4915,13 @@
         <v>70</v>
       </c>
       <c r="D64" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="E64" t="s">
         <v>721</v>
       </c>
       <c r="G64" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H64" t="s">
         <v>803</v>
@@ -4938,7 +4938,7 @@
         <v>721</v>
       </c>
       <c r="G65" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H65" t="s">
         <v>804</v>
@@ -4955,7 +4955,7 @@
         <v>721</v>
       </c>
       <c r="G66" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H66" t="s">
         <v>805</v>
@@ -4966,13 +4966,13 @@
         <v>73</v>
       </c>
       <c r="D67" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="E67" t="s">
         <v>721</v>
       </c>
       <c r="G67" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H67" t="s">
         <v>806</v>
@@ -4983,13 +4983,13 @@
         <v>74</v>
       </c>
       <c r="D68" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="E68" t="s">
         <v>721</v>
       </c>
       <c r="G68" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H68" t="s">
         <v>807</v>
@@ -5006,7 +5006,7 @@
         <v>721</v>
       </c>
       <c r="G69" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H69" t="s">
         <v>808</v>
@@ -5023,7 +5023,7 @@
         <v>721</v>
       </c>
       <c r="G70" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H70" t="s">
         <v>809</v>
@@ -5034,13 +5034,13 @@
         <v>77</v>
       </c>
       <c r="D71" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="E71" t="s">
         <v>721</v>
       </c>
       <c r="G71" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H71" t="s">
         <v>810</v>
@@ -5057,7 +5057,7 @@
         <v>721</v>
       </c>
       <c r="G72" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H72" t="s">
         <v>811</v>
@@ -5074,7 +5074,7 @@
         <v>427</v>
       </c>
       <c r="D73" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="E73" t="s">
         <v>721</v>
@@ -5083,10 +5083,10 @@
         <v>741</v>
       </c>
       <c r="G73" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H73" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -5100,7 +5100,7 @@
         <v>721</v>
       </c>
       <c r="G74" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="H74" t="s">
         <v>812</v>
@@ -5126,10 +5126,10 @@
         <v>741</v>
       </c>
       <c r="G75" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H75" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -5143,7 +5143,7 @@
         <v>722</v>
       </c>
       <c r="G76" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H76" t="s">
         <v>813</v>
@@ -5160,7 +5160,7 @@
         <v>722</v>
       </c>
       <c r="G77" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H77" t="s">
         <v>814</v>
@@ -5177,7 +5177,7 @@
         <v>722</v>
       </c>
       <c r="G78" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H78" t="s">
         <v>815</v>
@@ -5194,7 +5194,7 @@
         <v>722</v>
       </c>
       <c r="G79" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H79" t="s">
         <v>816</v>
@@ -5211,7 +5211,7 @@
         <v>722</v>
       </c>
       <c r="G80" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H80" t="s">
         <v>817</v>
@@ -5228,7 +5228,7 @@
         <v>722</v>
       </c>
       <c r="G81" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H81" t="s">
         <v>818</v>
@@ -5239,13 +5239,13 @@
         <v>88</v>
       </c>
       <c r="D82" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="E82" t="s">
         <v>722</v>
       </c>
       <c r="G82" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H82" t="s">
         <v>819</v>
@@ -5262,7 +5262,7 @@
         <v>722</v>
       </c>
       <c r="G83" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H83" t="s">
         <v>820</v>
@@ -5273,13 +5273,13 @@
         <v>90</v>
       </c>
       <c r="D84" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="E84" t="s">
         <v>722</v>
       </c>
       <c r="G84" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H84" t="s">
         <v>821</v>
@@ -5296,7 +5296,7 @@
         <v>722</v>
       </c>
       <c r="G85" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H85" t="s">
         <v>822</v>
@@ -5313,7 +5313,7 @@
         <v>722</v>
       </c>
       <c r="G86" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H86" t="s">
         <v>823</v>
@@ -5330,7 +5330,7 @@
         <v>722</v>
       </c>
       <c r="G87" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H87" t="s">
         <v>824</v>
@@ -5347,7 +5347,7 @@
         <v>722</v>
       </c>
       <c r="G88" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H88" t="s">
         <v>825</v>
@@ -5364,7 +5364,7 @@
         <v>722</v>
       </c>
       <c r="G89" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H89" t="s">
         <v>826</v>
@@ -5381,7 +5381,7 @@
         <v>722</v>
       </c>
       <c r="G90" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H90" t="s">
         <v>827</v>
@@ -5398,7 +5398,7 @@
         <v>722</v>
       </c>
       <c r="G91" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H91" t="s">
         <v>828</v>
@@ -5435,7 +5435,7 @@
         <v>722</v>
       </c>
       <c r="G93" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H93" t="s">
         <v>830</v>
@@ -5452,7 +5452,7 @@
         <v>723</v>
       </c>
       <c r="G94" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H94" t="s">
         <v>831</v>
@@ -5469,7 +5469,7 @@
         <v>723</v>
       </c>
       <c r="G95" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H95" t="s">
         <v>832</v>
@@ -5486,7 +5486,7 @@
         <v>723</v>
       </c>
       <c r="G96" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H96" t="s">
         <v>833</v>
@@ -5503,7 +5503,7 @@
         <v>723</v>
       </c>
       <c r="G97" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H97" t="s">
         <v>834</v>
@@ -5520,7 +5520,7 @@
         <v>723</v>
       </c>
       <c r="G98" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H98" t="s">
         <v>835</v>
@@ -5537,7 +5537,7 @@
         <v>723</v>
       </c>
       <c r="G99" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H99" t="s">
         <v>836</v>
@@ -5554,7 +5554,7 @@
         <v>723</v>
       </c>
       <c r="G100" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H100" t="s">
         <v>837</v>
@@ -5588,7 +5588,7 @@
         <v>723</v>
       </c>
       <c r="G102" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H102" t="s">
         <v>839</v>
@@ -5605,7 +5605,7 @@
         <v>723</v>
       </c>
       <c r="G103" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H103" t="s">
         <v>840</v>
@@ -5639,7 +5639,7 @@
         <v>723</v>
       </c>
       <c r="G105" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H105" t="s">
         <v>842</v>
@@ -5656,7 +5656,7 @@
         <v>723</v>
       </c>
       <c r="G106" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H106" t="s">
         <v>843</v>
@@ -5690,7 +5690,7 @@
         <v>427</v>
       </c>
       <c r="D108" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="E108" t="s">
         <v>723</v>
@@ -5699,10 +5699,10 @@
         <v>741</v>
       </c>
       <c r="G108" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H108" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="109" spans="1:8">
@@ -5716,7 +5716,7 @@
         <v>723</v>
       </c>
       <c r="G109" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H109" t="s">
         <v>845</v>
@@ -5767,7 +5767,7 @@
         <v>723</v>
       </c>
       <c r="G112" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H112" t="s">
         <v>848</v>
@@ -5778,7 +5778,7 @@
         <v>119</v>
       </c>
       <c r="D113" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="E113" t="s">
         <v>723</v>
@@ -5818,7 +5818,7 @@
         <v>723</v>
       </c>
       <c r="G115" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H115" t="s">
         <v>851</v>
@@ -5835,7 +5835,7 @@
         <v>724</v>
       </c>
       <c r="G116" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H116" t="s">
         <v>852</v>
@@ -5852,7 +5852,7 @@
         <v>724</v>
       </c>
       <c r="G117" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H117" t="s">
         <v>853</v>
@@ -5886,7 +5886,7 @@
         <v>427</v>
       </c>
       <c r="D119" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="E119" t="s">
         <v>724</v>
@@ -5895,10 +5895,10 @@
         <v>741</v>
       </c>
       <c r="G119" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H119" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="120" spans="1:8">
@@ -5912,7 +5912,7 @@
         <v>724</v>
       </c>
       <c r="G120" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H120" t="s">
         <v>855</v>
@@ -5923,13 +5923,13 @@
         <v>127</v>
       </c>
       <c r="D121" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="E121" t="s">
         <v>724</v>
       </c>
       <c r="G121" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H121" t="s">
         <v>856</v>
@@ -5946,7 +5946,7 @@
         <v>724</v>
       </c>
       <c r="G122" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H122" t="s">
         <v>857</v>
@@ -5963,7 +5963,7 @@
         <v>724</v>
       </c>
       <c r="G123" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H123" t="s">
         <v>858</v>
@@ -6031,7 +6031,7 @@
         <v>427</v>
       </c>
       <c r="D127" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="E127" t="s">
         <v>724</v>
@@ -6040,10 +6040,10 @@
         <v>741</v>
       </c>
       <c r="G127" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H127" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="128" spans="1:8">
@@ -6051,13 +6051,13 @@
         <v>134</v>
       </c>
       <c r="D128" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="E128" t="s">
         <v>724</v>
       </c>
       <c r="G128" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H128" t="s">
         <v>862</v>
@@ -6108,7 +6108,7 @@
         <v>726</v>
       </c>
       <c r="G131" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H131" t="s">
         <v>865</v>
@@ -6125,7 +6125,7 @@
         <v>726</v>
       </c>
       <c r="G132" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H132" t="s">
         <v>866</v>
@@ -6142,7 +6142,7 @@
         <v>726</v>
       </c>
       <c r="G133" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H133" t="s">
         <v>867</v>
@@ -6153,13 +6153,13 @@
         <v>140</v>
       </c>
       <c r="D134" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="E134" t="s">
         <v>726</v>
       </c>
       <c r="G134" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H134" t="s">
         <v>868</v>
@@ -6176,7 +6176,7 @@
         <v>726</v>
       </c>
       <c r="G135" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H135" t="s">
         <v>869</v>
@@ -6193,7 +6193,7 @@
         <v>726</v>
       </c>
       <c r="G136" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H136" t="s">
         <v>870</v>
@@ -6244,7 +6244,7 @@
         <v>726</v>
       </c>
       <c r="G139" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H139" t="s">
         <v>873</v>
@@ -6261,7 +6261,7 @@
         <v>726</v>
       </c>
       <c r="G140" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H140" t="s">
         <v>874</v>
@@ -6278,7 +6278,7 @@
         <v>726</v>
       </c>
       <c r="G141" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="H141" t="s">
         <v>875</v>
@@ -6329,7 +6329,7 @@
         <v>726</v>
       </c>
       <c r="G144" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H144" t="s">
         <v>878</v>
@@ -6346,7 +6346,7 @@
         <v>726</v>
       </c>
       <c r="G145" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="H145" t="s">
         <v>879</v>
@@ -6363,7 +6363,7 @@
         <v>726</v>
       </c>
       <c r="G146" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="H146" t="s">
         <v>880</v>
@@ -6380,7 +6380,7 @@
         <v>726</v>
       </c>
       <c r="G147" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H147" t="s">
         <v>881</v>
@@ -6414,7 +6414,7 @@
         <v>726</v>
       </c>
       <c r="G149" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H149" t="s">
         <v>883</v>
@@ -6448,7 +6448,7 @@
         <v>726</v>
       </c>
       <c r="G151" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H151" t="s">
         <v>885</v>
@@ -6465,7 +6465,7 @@
         <v>727</v>
       </c>
       <c r="G152" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H152" t="s">
         <v>886</v>
@@ -6482,7 +6482,7 @@
         <v>727</v>
       </c>
       <c r="G153" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H153" t="s">
         <v>887</v>
@@ -6499,7 +6499,7 @@
         <v>727</v>
       </c>
       <c r="G154" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H154" t="s">
         <v>888</v>
@@ -6516,7 +6516,7 @@
         <v>727</v>
       </c>
       <c r="G155" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H155" t="s">
         <v>889</v>
@@ -6533,7 +6533,7 @@
         <v>727</v>
       </c>
       <c r="G156" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H156" t="s">
         <v>890</v>
@@ -6550,7 +6550,7 @@
         <v>727</v>
       </c>
       <c r="G157" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H157" t="s">
         <v>891</v>
@@ -6567,7 +6567,7 @@
         <v>727</v>
       </c>
       <c r="G158" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H158" t="s">
         <v>892</v>
@@ -6584,7 +6584,7 @@
         <v>727</v>
       </c>
       <c r="G159" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="H159" t="s">
         <v>893</v>
@@ -6601,7 +6601,7 @@
         <v>727</v>
       </c>
       <c r="G160" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H160" t="s">
         <v>894</v>
@@ -6630,7 +6630,7 @@
         <v>748</v>
       </c>
       <c r="H161" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="162" spans="1:8">
@@ -6644,7 +6644,7 @@
         <v>727</v>
       </c>
       <c r="G162" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H162" t="s">
         <v>895</v>
@@ -6695,7 +6695,7 @@
         <v>727</v>
       </c>
       <c r="G165" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H165" t="s">
         <v>898</v>
@@ -6763,7 +6763,7 @@
         <v>727</v>
       </c>
       <c r="G169" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H169" t="s">
         <v>902</v>
@@ -6843,7 +6843,7 @@
         <v>748</v>
       </c>
       <c r="H173" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="174" spans="1:8">
@@ -6857,7 +6857,7 @@
         <v>728</v>
       </c>
       <c r="G174" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H174" t="s">
         <v>906</v>
@@ -6874,7 +6874,7 @@
         <v>728</v>
       </c>
       <c r="G175" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H175" t="s">
         <v>907</v>
@@ -6905,13 +6905,13 @@
         <v>426</v>
       </c>
       <c r="D177" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="E177" t="s">
         <v>723</v>
       </c>
       <c r="G177" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H177" t="s">
         <v>909</v>
@@ -6928,7 +6928,7 @@
         <v>728</v>
       </c>
       <c r="G178" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H178" t="s">
         <v>910</v>
@@ -6979,7 +6979,7 @@
         <v>728</v>
       </c>
       <c r="G181" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H181" t="s">
         <v>913</v>
@@ -6996,7 +6996,7 @@
         <v>728</v>
       </c>
       <c r="G182" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H182" t="s">
         <v>914</v>
@@ -7025,7 +7025,7 @@
         <v>748</v>
       </c>
       <c r="H183" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="184" spans="1:8">
@@ -7056,7 +7056,7 @@
         <v>728</v>
       </c>
       <c r="G185" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H185" t="s">
         <v>916</v>
@@ -7158,7 +7158,7 @@
         <v>728</v>
       </c>
       <c r="G191" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H191" t="s">
         <v>922</v>
@@ -7175,7 +7175,7 @@
         <v>729</v>
       </c>
       <c r="G192" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H192" t="s">
         <v>923</v>
@@ -7192,7 +7192,7 @@
         <v>729</v>
       </c>
       <c r="G193" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H193" t="s">
         <v>924</v>
@@ -7209,7 +7209,7 @@
         <v>729</v>
       </c>
       <c r="G194" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H194" t="s">
         <v>925</v>
@@ -7226,7 +7226,7 @@
         <v>729</v>
       </c>
       <c r="G195" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H195" t="s">
         <v>926</v>
@@ -7243,7 +7243,7 @@
         <v>729</v>
       </c>
       <c r="G196" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H196" t="s">
         <v>927</v>
@@ -7260,7 +7260,7 @@
         <v>729</v>
       </c>
       <c r="G197" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H197" t="s">
         <v>928</v>
@@ -7311,7 +7311,7 @@
         <v>729</v>
       </c>
       <c r="G200" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H200" t="s">
         <v>931</v>
@@ -7362,7 +7362,7 @@
         <v>729</v>
       </c>
       <c r="G203" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H203" t="s">
         <v>934</v>
@@ -7396,7 +7396,7 @@
         <v>729</v>
       </c>
       <c r="G205" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H205" t="s">
         <v>936</v>
@@ -7413,7 +7413,7 @@
         <v>729</v>
       </c>
       <c r="G206" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H206" t="s">
         <v>937</v>
@@ -7532,7 +7532,7 @@
         <v>729</v>
       </c>
       <c r="G213" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="H213" t="s">
         <v>944</v>
@@ -7566,7 +7566,7 @@
         <v>729</v>
       </c>
       <c r="G215" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="H215" t="s">
         <v>946</v>
@@ -7583,7 +7583,7 @@
         <v>730</v>
       </c>
       <c r="G216" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H216" t="s">
         <v>947</v>
@@ -7593,17 +7593,26 @@
       <c r="A217" t="s">
         <v>223</v>
       </c>
+      <c r="B217" t="s">
+        <v>426</v>
+      </c>
+      <c r="C217" t="s">
+        <v>427</v>
+      </c>
       <c r="D217" t="s">
         <v>577</v>
       </c>
       <c r="E217" t="s">
-        <v>730</v>
+        <v>731</v>
+      </c>
+      <c r="F217" t="s">
+        <v>741</v>
       </c>
       <c r="G217" t="s">
-        <v>749</v>
+        <v>744</v>
       </c>
       <c r="H217" t="s">
-        <v>948</v>
+        <v>753</v>
       </c>
     </row>
     <row r="218" spans="1:8">
@@ -7614,13 +7623,13 @@
         <v>578</v>
       </c>
       <c r="E218" t="s">
-        <v>730</v>
+        <v>717</v>
       </c>
       <c r="G218" t="s">
-        <v>749</v>
+        <v>744</v>
       </c>
       <c r="H218" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="219" spans="1:8">
@@ -7631,39 +7640,30 @@
         <v>579</v>
       </c>
       <c r="E219" t="s">
-        <v>730</v>
+        <v>717</v>
       </c>
       <c r="G219" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="H219" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="220" spans="1:8">
       <c r="A220" t="s">
         <v>226</v>
       </c>
-      <c r="B220" t="s">
-        <v>426</v>
-      </c>
-      <c r="C220" t="s">
-        <v>427</v>
-      </c>
       <c r="D220" t="s">
         <v>580</v>
       </c>
       <c r="E220" t="s">
-        <v>731</v>
-      </c>
-      <c r="F220" t="s">
-        <v>741</v>
+        <v>717</v>
       </c>
       <c r="G220" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H220" t="s">
-        <v>752</v>
+        <v>950</v>
       </c>
     </row>
     <row r="221" spans="1:8">
@@ -7674,10 +7674,10 @@
         <v>581</v>
       </c>
       <c r="E221" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="G221" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="H221" t="s">
         <v>951</v>
@@ -7688,13 +7688,13 @@
         <v>228</v>
       </c>
       <c r="D222" t="s">
-        <v>582</v>
+        <v>495</v>
       </c>
       <c r="E222" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="G222" t="s">
-        <v>749</v>
+        <v>744</v>
       </c>
       <c r="H222" t="s">
         <v>952</v>
@@ -7705,13 +7705,13 @@
         <v>229</v>
       </c>
       <c r="D223" t="s">
-        <v>583</v>
+        <v>496</v>
       </c>
       <c r="E223" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="G223" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="H223" t="s">
         <v>953</v>
@@ -7722,10 +7722,10 @@
         <v>230</v>
       </c>
       <c r="D224" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="E224" t="s">
-        <v>720</v>
+        <v>730</v>
       </c>
       <c r="G224" t="s">
         <v>749</v>
@@ -7739,13 +7739,13 @@
         <v>231</v>
       </c>
       <c r="D225" t="s">
-        <v>495</v>
+        <v>583</v>
       </c>
       <c r="E225" t="s">
-        <v>720</v>
+        <v>730</v>
       </c>
       <c r="G225" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="H225" t="s">
         <v>955</v>
@@ -7756,13 +7756,13 @@
         <v>232</v>
       </c>
       <c r="D226" t="s">
-        <v>496</v>
+        <v>584</v>
       </c>
       <c r="E226" t="s">
-        <v>720</v>
+        <v>730</v>
       </c>
       <c r="G226" t="s">
-        <v>749</v>
+        <v>744</v>
       </c>
       <c r="H226" t="s">
         <v>956</v>
@@ -7830,7 +7830,7 @@
         <v>730</v>
       </c>
       <c r="G230" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H230" t="s">
         <v>960</v>
@@ -7966,7 +7966,7 @@
         <v>730</v>
       </c>
       <c r="G238" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H238" t="s">
         <v>968</v>
@@ -8026,10 +8026,10 @@
         <v>743</v>
       </c>
       <c r="G241" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H241" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="242" spans="1:8">
@@ -8055,7 +8055,7 @@
         <v>749</v>
       </c>
       <c r="H242" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="243" spans="1:8">
@@ -8069,7 +8069,7 @@
         <v>730</v>
       </c>
       <c r="G243" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="H243" t="s">
         <v>971</v>
@@ -8086,7 +8086,7 @@
         <v>730</v>
       </c>
       <c r="G244" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="H244" t="s">
         <v>972</v>
@@ -8106,7 +8106,7 @@
         <v>749</v>
       </c>
       <c r="H245" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
     </row>
     <row r="246" spans="1:8">
@@ -8154,7 +8154,7 @@
         <v>730</v>
       </c>
       <c r="G248" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="H248" t="s">
         <v>975</v>
@@ -8200,7 +8200,7 @@
         <v>748</v>
       </c>
       <c r="H250" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="251" spans="1:8">
@@ -8231,7 +8231,7 @@
         <v>732</v>
       </c>
       <c r="G252" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H252" t="s">
         <v>978</v>
@@ -8265,7 +8265,7 @@
         <v>732</v>
       </c>
       <c r="G254" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="H254" t="s">
         <v>980</v>
@@ -8282,7 +8282,7 @@
         <v>732</v>
       </c>
       <c r="G255" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="H255" t="s">
         <v>981</v>
@@ -8299,7 +8299,7 @@
         <v>732</v>
       </c>
       <c r="G256" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="H256" t="s">
         <v>982</v>
@@ -8328,7 +8328,7 @@
         <v>748</v>
       </c>
       <c r="H257" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="258" spans="1:8">
@@ -8342,7 +8342,7 @@
         <v>732</v>
       </c>
       <c r="G258" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="H258" t="s">
         <v>983</v>
@@ -8371,7 +8371,7 @@
         <v>748</v>
       </c>
       <c r="H259" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="260" spans="1:8">
@@ -8385,7 +8385,7 @@
         <v>732</v>
       </c>
       <c r="G260" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="H260" t="s">
         <v>984</v>
@@ -8453,7 +8453,7 @@
         <v>733</v>
       </c>
       <c r="G264" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="H264" t="s">
         <v>988</v>
@@ -8470,7 +8470,7 @@
         <v>733</v>
       </c>
       <c r="G265" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="H265" t="s">
         <v>989</v>
@@ -8487,7 +8487,7 @@
         <v>733</v>
       </c>
       <c r="G266" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="H266" t="s">
         <v>990</v>
@@ -8504,7 +8504,7 @@
         <v>733</v>
       </c>
       <c r="G267" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="H267" t="s">
         <v>991</v>
@@ -8521,7 +8521,7 @@
         <v>733</v>
       </c>
       <c r="G268" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="H268" t="s">
         <v>992</v>
@@ -8538,7 +8538,7 @@
         <v>734</v>
       </c>
       <c r="G269" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H269" t="s">
         <v>993</v>
@@ -8640,7 +8640,7 @@
         <v>734</v>
       </c>
       <c r="G275" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H275" t="s">
         <v>999</v>
@@ -8657,7 +8657,7 @@
         <v>734</v>
       </c>
       <c r="G276" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H276" t="s">
         <v>1000</v>
@@ -8708,7 +8708,7 @@
         <v>734</v>
       </c>
       <c r="G279" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H279" t="s">
         <v>1003</v>
@@ -8813,7 +8813,7 @@
         <v>748</v>
       </c>
       <c r="H285" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
     </row>
     <row r="286" spans="1:8">
@@ -8873,7 +8873,7 @@
         <v>749</v>
       </c>
       <c r="H288" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="289" spans="1:8">
@@ -8899,7 +8899,7 @@
         <v>749</v>
       </c>
       <c r="H289" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="290" spans="1:8">
@@ -9146,10 +9146,10 @@
         <v>741</v>
       </c>
       <c r="G303" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H303" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="304" spans="1:8">
@@ -9163,7 +9163,7 @@
         <v>736</v>
       </c>
       <c r="G304" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H304" t="s">
         <v>1024</v>
@@ -9192,7 +9192,7 @@
         <v>749</v>
       </c>
       <c r="H305" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="306" spans="1:8">
@@ -9218,7 +9218,7 @@
         <v>749</v>
       </c>
       <c r="H306" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="307" spans="1:8">
@@ -9249,7 +9249,7 @@
         <v>736</v>
       </c>
       <c r="G308" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H308" t="s">
         <v>1026</v>
@@ -9300,7 +9300,7 @@
         <v>736</v>
       </c>
       <c r="G311" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H311" t="s">
         <v>1029</v>
@@ -9329,7 +9329,7 @@
         <v>748</v>
       </c>
       <c r="H312" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="313" spans="1:8">
@@ -9369,10 +9369,10 @@
         <v>741</v>
       </c>
       <c r="G314" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H314" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="315" spans="1:8">
@@ -9386,7 +9386,7 @@
         <v>736</v>
       </c>
       <c r="G315" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H315" t="s">
         <v>1031</v>
@@ -9432,7 +9432,7 @@
         <v>749</v>
       </c>
       <c r="H317" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="318" spans="1:8">
@@ -9446,7 +9446,7 @@
         <v>736</v>
       </c>
       <c r="G318" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H318" t="s">
         <v>1033</v>
@@ -9475,7 +9475,7 @@
         <v>749</v>
       </c>
       <c r="H319" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="320" spans="1:8">
@@ -9506,7 +9506,7 @@
         <v>736</v>
       </c>
       <c r="G321" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H321" t="s">
         <v>1035</v>
@@ -9535,7 +9535,7 @@
         <v>748</v>
       </c>
       <c r="H322" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="323" spans="1:8">
@@ -9549,7 +9549,7 @@
         <v>736</v>
       </c>
       <c r="G323" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H323" t="s">
         <v>1036</v>
@@ -9595,7 +9595,7 @@
         <v>749</v>
       </c>
       <c r="H325" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="326" spans="1:8">
@@ -9621,7 +9621,7 @@
         <v>749</v>
       </c>
       <c r="H326" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="327" spans="1:8">
@@ -9647,7 +9647,7 @@
         <v>749</v>
       </c>
       <c r="H327" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="328" spans="1:8">
@@ -9661,7 +9661,7 @@
         <v>736</v>
       </c>
       <c r="G328" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H328" t="s">
         <v>1038</v>
@@ -9763,7 +9763,7 @@
         <v>736</v>
       </c>
       <c r="G334" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H334" t="s">
         <v>1043</v>
@@ -9882,7 +9882,7 @@
         <v>737</v>
       </c>
       <c r="G341" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H341" t="s">
         <v>1050</v>
@@ -9908,10 +9908,10 @@
         <v>741</v>
       </c>
       <c r="G342" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H342" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="343" spans="1:8">
@@ -9925,7 +9925,7 @@
         <v>737</v>
       </c>
       <c r="G343" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H343" t="s">
         <v>1051</v>
@@ -10010,7 +10010,7 @@
         <v>737</v>
       </c>
       <c r="G348" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="H348" t="s">
         <v>1056</v>
@@ -10036,10 +10036,10 @@
         <v>741</v>
       </c>
       <c r="G349" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H349" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="350" spans="1:8">
@@ -10062,10 +10062,10 @@
         <v>741</v>
       </c>
       <c r="G350" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H350" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="351" spans="1:8">
@@ -10079,7 +10079,7 @@
         <v>737</v>
       </c>
       <c r="G351" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H351" t="s">
         <v>1057</v>
@@ -10249,7 +10249,7 @@
         <v>738</v>
       </c>
       <c r="G361" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H361" t="s">
         <v>1026</v>
@@ -10326,10 +10326,10 @@
         <v>741</v>
       </c>
       <c r="G365" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H365" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="366" spans="1:8">
@@ -10343,7 +10343,7 @@
         <v>738</v>
       </c>
       <c r="G366" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H366" t="s">
         <v>1070</v>
@@ -10394,7 +10394,7 @@
         <v>738</v>
       </c>
       <c r="G369" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H369" t="s">
         <v>1073</v>
@@ -10632,7 +10632,7 @@
         <v>739</v>
       </c>
       <c r="G383" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="H383" t="s">
         <v>1087</v>
@@ -10717,7 +10717,7 @@
         <v>739</v>
       </c>
       <c r="G388" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H388" t="s">
         <v>1092</v>
@@ -10734,7 +10734,7 @@
         <v>739</v>
       </c>
       <c r="G389" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H389" t="s">
         <v>1093</v>
@@ -10751,7 +10751,7 @@
         <v>739</v>
       </c>
       <c r="G390" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H390" t="s">
         <v>1094</v>
@@ -10768,7 +10768,7 @@
         <v>739</v>
       </c>
       <c r="G391" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H391" t="s">
         <v>1095</v>
@@ -10785,7 +10785,7 @@
         <v>739</v>
       </c>
       <c r="G392" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H392" t="s">
         <v>1096</v>
@@ -10802,7 +10802,7 @@
         <v>739</v>
       </c>
       <c r="G393" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H393" t="s">
         <v>1097</v>
@@ -10819,7 +10819,7 @@
         <v>739</v>
       </c>
       <c r="G394" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H394" t="s">
         <v>1098</v>
@@ -10845,10 +10845,10 @@
         <v>741</v>
       </c>
       <c r="G395" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H395" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="396" spans="1:8">
@@ -10862,7 +10862,7 @@
         <v>739</v>
       </c>
       <c r="G396" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H396" t="s">
         <v>1099</v>
@@ -10879,7 +10879,7 @@
         <v>739</v>
       </c>
       <c r="G397" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H397" t="s">
         <v>1100</v>
@@ -10925,7 +10925,7 @@
         <v>748</v>
       </c>
       <c r="H399" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="400" spans="1:8">
@@ -10951,7 +10951,7 @@
         <v>748</v>
       </c>
       <c r="H400" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="401" spans="1:8">
@@ -10965,7 +10965,7 @@
         <v>740</v>
       </c>
       <c r="G401" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="H401" t="s">
         <v>1102</v>
@@ -10982,7 +10982,7 @@
         <v>731</v>
       </c>
       <c r="G402" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H402" t="s">
         <v>1103</v>
@@ -11016,7 +11016,7 @@
         <v>731</v>
       </c>
       <c r="G404" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H404" t="s">
         <v>1105</v>
@@ -11033,7 +11033,7 @@
         <v>731</v>
       </c>
       <c r="G405" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H405" t="s">
         <v>1106</v>
@@ -11050,7 +11050,7 @@
         <v>731</v>
       </c>
       <c r="G406" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H406" t="s">
         <v>1107</v>
@@ -11067,7 +11067,7 @@
         <v>731</v>
       </c>
       <c r="G407" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H407" t="s">
         <v>1108</v>
@@ -11130,7 +11130,7 @@
         <v>749</v>
       </c>
       <c r="H410" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="411" spans="1:8">
@@ -11161,7 +11161,7 @@
         <v>731</v>
       </c>
       <c r="G412" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="H412" t="s">
         <v>1112</v>
@@ -11195,7 +11195,7 @@
         <v>731</v>
       </c>
       <c r="G414" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H414" t="s">
         <v>1114</v>

</xml_diff>